<commit_message>
Changed People to proper roles, will hand off to PMs for more massaging
</commit_message>
<xml_diff>
--- a/mac-low/OLR/xls_standard_input_mac_low.xlsx
+++ b/mac-low/OLR/xls_standard_input_mac_low.xlsx
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5828" uniqueCount="2204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5827" uniqueCount="2204">
   <si>
     <t>text</t>
   </si>
@@ -7925,10 +7925,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R488"/>
+  <dimension ref="A1:Q488"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7946,10 +7946,9 @@
     <col min="13" max="13" width="15.140625" style="3" customWidth="1"/>
     <col min="14" max="14" width="82" style="3" customWidth="1"/>
     <col min="15" max="17" width="39.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="42.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -7973,10 +7972,10 @@
         <v>1</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>516</v>
+        <v>96</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>517</v>
+        <v>247</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>487</v>
@@ -7999,11 +7998,8 @@
       <c r="Q1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>1519</v>
       </c>
@@ -8048,7 +8044,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>1002</v>
       </c>
@@ -8090,7 +8086,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>1002</v>
       </c>
@@ -8124,7 +8120,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>1002</v>
       </c>
@@ -8158,7 +8154,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>1003</v>
       </c>
@@ -8200,7 +8196,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>1003</v>
       </c>
@@ -8234,7 +8230,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>1003</v>
       </c>
@@ -8268,7 +8264,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>1004</v>
       </c>
@@ -8310,7 +8306,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>1004</v>
       </c>
@@ -8344,7 +8340,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>1004</v>
       </c>
@@ -8378,7 +8374,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>1005</v>
       </c>
@@ -8420,7 +8416,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>1006</v>
       </c>
@@ -8459,7 +8455,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>1006</v>
       </c>
@@ -8493,7 +8489,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>1006</v>
       </c>
@@ -8527,7 +8523,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>1007</v>
       </c>
@@ -9132,7 +9128,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <v>1014</v>
       </c>
@@ -9174,7 +9170,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>1015</v>
       </c>
@@ -9213,7 +9209,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <v>1015</v>
       </c>
@@ -9247,7 +9243,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>1015</v>
       </c>
@@ -9281,7 +9277,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
         <v>1016</v>
       </c>
@@ -9323,7 +9319,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>1017</v>
       </c>
@@ -9346,6 +9342,9 @@
       <c r="H38" t="s">
         <v>646</v>
       </c>
+      <c r="J38" s="3" t="s">
+        <v>2184</v>
+      </c>
       <c r="K38" t="s">
         <v>925</v>
       </c>
@@ -9361,11 +9360,8 @@
       <c r="Q38" s="3" t="s">
         <v>1342</v>
       </c>
-      <c r="R38" s="3" t="s">
-        <v>2184</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <v>1017</v>
       </c>
@@ -9399,7 +9395,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>1017</v>
       </c>
@@ -9433,7 +9429,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
         <v>1018</v>
       </c>
@@ -9472,7 +9468,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>1018</v>
       </c>
@@ -9506,7 +9502,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="22">
         <v>1018</v>
       </c>
@@ -9540,7 +9536,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>1019</v>
       </c>
@@ -9582,7 +9578,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
         <v>1019</v>
       </c>
@@ -9616,7 +9612,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
         <v>1019</v>
       </c>
@@ -9650,7 +9646,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="22">
         <v>1020</v>
       </c>
@@ -9673,6 +9669,9 @@
       <c r="H47" t="s">
         <v>649</v>
       </c>
+      <c r="J47" s="3" t="s">
+        <v>2185</v>
+      </c>
       <c r="K47" t="s">
         <v>928</v>
       </c>
@@ -9691,11 +9690,8 @@
       <c r="Q47" s="3" t="s">
         <v>1345</v>
       </c>
-      <c r="R47" s="3" t="s">
-        <v>2185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
         <v>1021</v>
       </c>
@@ -9718,6 +9714,9 @@
       <c r="H48" t="s">
         <v>650</v>
       </c>
+      <c r="J48" s="3" t="s">
+        <v>2186</v>
+      </c>
       <c r="K48" t="s">
         <v>929</v>
       </c>
@@ -9735,9 +9734,6 @@
       </c>
       <c r="Q48" s="3" t="s">
         <v>1346</v>
-      </c>
-      <c r="R48" s="3" t="s">
-        <v>2186</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -11509,7 +11505,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="22">
         <v>1038</v>
       </c>
@@ -11551,7 +11547,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="22">
         <v>1039</v>
       </c>
@@ -11593,7 +11589,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="22">
         <v>1040</v>
       </c>
@@ -11635,7 +11631,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="22">
         <v>1041</v>
       </c>
@@ -11677,7 +11673,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="22">
         <v>1042</v>
       </c>
@@ -11719,7 +11715,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="22">
         <v>1043</v>
       </c>
@@ -11764,7 +11760,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="22">
         <v>1044</v>
       </c>
@@ -11806,7 +11802,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="22">
         <v>1045</v>
       </c>
@@ -11848,7 +11844,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="22">
         <v>1046</v>
       </c>
@@ -11871,6 +11867,9 @@
       <c r="H105" t="s">
         <v>675</v>
       </c>
+      <c r="J105" s="3" t="s">
+        <v>2187</v>
+      </c>
       <c r="K105" t="s">
         <v>942</v>
       </c>
@@ -11889,11 +11888,8 @@
       <c r="Q105" s="3" t="s">
         <v>1371</v>
       </c>
-      <c r="R105" s="3" t="s">
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="22">
         <v>1047</v>
       </c>
@@ -11935,7 +11931,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="22">
         <v>1048</v>
       </c>
@@ -11977,7 +11973,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="22">
         <v>1048</v>
       </c>
@@ -12011,7 +12007,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="22">
         <v>1048</v>
       </c>
@@ -12045,7 +12041,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="22">
         <v>1049</v>
       </c>
@@ -12087,7 +12083,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="22">
         <v>1049</v>
       </c>
@@ -12121,7 +12117,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="22">
         <v>1049</v>
       </c>
@@ -12155,7 +12151,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="22">
         <v>1049</v>
       </c>
@@ -12189,7 +12185,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="22">
         <v>1049</v>
       </c>
@@ -12223,7 +12219,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="22">
         <v>1050</v>
       </c>
@@ -12268,7 +12264,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="22">
         <v>1050</v>
       </c>
@@ -12302,7 +12298,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="22">
         <v>1050</v>
       </c>
@@ -12336,7 +12332,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="22">
         <v>1051</v>
       </c>
@@ -12381,7 +12377,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="22">
         <v>1051</v>
       </c>
@@ -12415,7 +12411,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="22">
         <v>1051</v>
       </c>
@@ -12449,7 +12445,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="22">
         <v>1052</v>
       </c>
@@ -12472,6 +12468,9 @@
       <c r="H121" t="s">
         <v>681</v>
       </c>
+      <c r="J121" s="3" t="s">
+        <v>2188</v>
+      </c>
       <c r="K121" t="s">
         <v>945</v>
       </c>
@@ -12493,11 +12492,8 @@
       <c r="Q121" s="3" t="s">
         <v>1377</v>
       </c>
-      <c r="R121" s="3" t="s">
-        <v>2188</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
         <v>1052</v>
       </c>
@@ -12531,7 +12527,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="22">
         <v>1052</v>
       </c>
@@ -12565,7 +12561,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="22">
         <v>1053</v>
       </c>
@@ -12607,7 +12603,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="22">
         <v>1053</v>
       </c>
@@ -12641,7 +12637,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
         <v>1053</v>
       </c>
@@ -12675,7 +12671,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="22">
         <v>1054</v>
       </c>
@@ -12717,7 +12713,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
         <v>1054</v>
       </c>
@@ -12751,7 +12747,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="22">
         <v>1054</v>
       </c>
@@ -12785,7 +12781,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
         <v>1055</v>
       </c>
@@ -12827,7 +12823,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="22">
         <v>1055</v>
       </c>
@@ -12861,7 +12857,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
         <v>1055</v>
       </c>
@@ -12895,7 +12891,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="22">
         <v>1056</v>
       </c>
@@ -12929,7 +12925,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
         <v>1056</v>
       </c>
@@ -12957,7 +12953,7 @@
       <c r="M134" s="23"/>
       <c r="O134"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
         <v>1056</v>
       </c>
@@ -12985,7 +12981,7 @@
       <c r="M135" s="23"/>
       <c r="O135"/>
     </row>
-    <row r="136" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
         <v>1057</v>
       </c>
@@ -12999,6 +12995,9 @@
       <c r="H136" t="s">
         <v>686</v>
       </c>
+      <c r="J136" s="3" t="s">
+        <v>2189</v>
+      </c>
       <c r="K136" t="s">
         <v>946</v>
       </c>
@@ -13017,11 +13016,8 @@
       <c r="Q136" s="3" t="s">
         <v>1382</v>
       </c>
-      <c r="R136" s="3" t="s">
-        <v>2189</v>
-      </c>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="22">
         <v>1057</v>
       </c>
@@ -13049,7 +13045,7 @@
       <c r="M137" s="23"/>
       <c r="O137"/>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
         <v>1057</v>
       </c>
@@ -13077,7 +13073,7 @@
       <c r="M138" s="23"/>
       <c r="O138"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="22">
         <v>1058</v>
       </c>
@@ -13119,7 +13115,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="22">
         <v>1059</v>
       </c>
@@ -13158,7 +13154,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="22">
         <v>1059</v>
       </c>
@@ -13192,7 +13188,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
         <v>1059</v>
       </c>
@@ -13226,7 +13222,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="22">
         <v>1060</v>
       </c>
@@ -13249,6 +13245,9 @@
       <c r="H143" t="s">
         <v>689</v>
       </c>
+      <c r="J143" s="3" t="s">
+        <v>2190</v>
+      </c>
       <c r="K143" t="s">
         <v>949</v>
       </c>
@@ -13270,11 +13269,8 @@
       <c r="Q143" s="3" t="s">
         <v>1384</v>
       </c>
-      <c r="R143" s="3" t="s">
-        <v>2190</v>
-      </c>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="22">
         <v>1061</v>
       </c>
@@ -13297,6 +13293,9 @@
       <c r="H144" t="s">
         <v>690</v>
       </c>
+      <c r="J144" s="3" t="s">
+        <v>2190</v>
+      </c>
       <c r="K144" t="s">
         <v>949</v>
       </c>
@@ -13317,9 +13316,6 @@
       </c>
       <c r="Q144" s="3" t="s">
         <v>1385</v>
-      </c>
-      <c r="R144" s="3" t="s">
-        <v>2190</v>
       </c>
     </row>
     <row r="145" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -14522,7 +14518,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" s="22">
         <v>1079</v>
       </c>
@@ -14556,7 +14552,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A178" s="22">
         <v>1079</v>
       </c>
@@ -14590,7 +14586,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="179" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="22">
         <v>1080</v>
       </c>
@@ -14632,7 +14628,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A180" s="22">
         <v>1081</v>
       </c>
@@ -14674,7 +14670,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="181" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="22">
         <v>1082</v>
       </c>
@@ -14697,6 +14693,9 @@
       <c r="H181" t="s">
         <v>705</v>
       </c>
+      <c r="J181" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="K181" t="s">
         <v>966</v>
       </c>
@@ -14715,11 +14714,8 @@
       <c r="Q181" s="3" t="s">
         <v>1399</v>
       </c>
-      <c r="R181" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="182" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="22">
         <v>1083</v>
       </c>
@@ -14742,6 +14738,9 @@
       <c r="H182" t="s">
         <v>706</v>
       </c>
+      <c r="J182" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="K182" t="s">
         <v>966</v>
       </c>
@@ -14760,11 +14759,8 @@
       <c r="Q182" s="3" t="s">
         <v>1400</v>
       </c>
-      <c r="R182" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="183" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="22">
         <v>1084</v>
       </c>
@@ -14787,6 +14783,9 @@
       <c r="H183" t="s">
         <v>707</v>
       </c>
+      <c r="J183" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="K183" t="s">
         <v>966</v>
       </c>
@@ -14805,11 +14804,8 @@
       <c r="Q183" s="3" t="s">
         <v>1401</v>
       </c>
-      <c r="R183" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="22">
         <v>1085</v>
       </c>
@@ -14832,6 +14828,9 @@
       <c r="H184" t="s">
         <v>708</v>
       </c>
+      <c r="J184" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="K184" t="s">
         <v>966</v>
       </c>
@@ -14850,11 +14849,8 @@
       <c r="Q184" s="3" t="s">
         <v>1402</v>
       </c>
-      <c r="R184" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="185" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="22">
         <v>1086</v>
       </c>
@@ -14877,6 +14873,9 @@
       <c r="H185" t="s">
         <v>709</v>
       </c>
+      <c r="J185" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="K185" t="s">
         <v>966</v>
       </c>
@@ -14895,11 +14894,8 @@
       <c r="Q185" s="3" t="s">
         <v>1403</v>
       </c>
-      <c r="R185" s="3" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A186" s="22">
         <v>1087</v>
       </c>
@@ -14941,7 +14937,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" s="22">
         <v>1087</v>
       </c>
@@ -14975,7 +14971,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A188" s="22">
         <v>1087</v>
       </c>
@@ -15009,7 +15005,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A189" s="22">
         <v>1088</v>
       </c>
@@ -15051,7 +15047,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" s="22">
         <v>1088</v>
       </c>
@@ -15085,7 +15081,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A191" s="22">
         <v>1088</v>
       </c>
@@ -15119,7 +15115,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A192" s="22">
         <v>1089</v>
       </c>
@@ -15161,7 +15157,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A193" s="22">
         <v>1090</v>
       </c>
@@ -15203,7 +15199,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A194" s="22">
         <v>1091</v>
       </c>
@@ -15242,7 +15238,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A195" s="22">
         <v>1092</v>
       </c>
@@ -15281,7 +15277,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="196" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="22">
         <v>1093</v>
       </c>
@@ -15323,7 +15319,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A197" s="22">
         <v>1094</v>
       </c>
@@ -15346,6 +15342,9 @@
       <c r="H197" t="s">
         <v>717</v>
       </c>
+      <c r="J197" s="3" t="s">
+        <v>2192</v>
+      </c>
       <c r="K197" t="s">
         <v>972</v>
       </c>
@@ -15364,11 +15363,8 @@
       <c r="P197" s="3" t="s">
         <v>1303</v>
       </c>
-      <c r="R197" s="3" t="s">
-        <v>2192</v>
-      </c>
-    </row>
-    <row r="198" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="22">
         <v>1095</v>
       </c>
@@ -15410,7 +15406,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="199" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="22">
         <v>1096</v>
       </c>
@@ -15433,6 +15429,9 @@
       <c r="H199" t="s">
         <v>719</v>
       </c>
+      <c r="J199" s="3" t="s">
+        <v>2189</v>
+      </c>
       <c r="K199" t="s">
         <v>974</v>
       </c>
@@ -15451,11 +15450,8 @@
       <c r="Q199" s="3" t="s">
         <v>1411</v>
       </c>
-      <c r="R199" s="3" t="s">
-        <v>2189</v>
-      </c>
-    </row>
-    <row r="200" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A200" s="22">
         <v>1097</v>
       </c>
@@ -15497,7 +15493,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="201" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="22">
         <v>1098</v>
       </c>
@@ -15539,7 +15535,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A202" s="22">
         <v>1099</v>
       </c>
@@ -15581,7 +15577,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A203" s="22">
         <v>1099</v>
       </c>
@@ -15615,7 +15611,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" s="22">
         <v>1099</v>
       </c>
@@ -15649,7 +15645,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="22">
         <v>1100</v>
       </c>
@@ -15672,6 +15668,9 @@
       <c r="H205" t="s">
         <v>723</v>
       </c>
+      <c r="J205" s="3" t="s">
+        <v>2192</v>
+      </c>
       <c r="K205" t="s">
         <v>977</v>
       </c>
@@ -15690,11 +15689,8 @@
       <c r="Q205" s="3" t="s">
         <v>1415</v>
       </c>
-      <c r="R205" s="3" t="s">
-        <v>2192</v>
-      </c>
-    </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A206" s="22">
         <v>1100</v>
       </c>
@@ -15728,7 +15724,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" s="22">
         <v>1100</v>
       </c>
@@ -15762,7 +15758,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A208" s="22">
         <v>1101</v>
       </c>
@@ -16460,7 +16456,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A225" s="22">
         <v>1116</v>
       </c>
@@ -16499,7 +16495,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" s="22">
         <v>1117</v>
       </c>
@@ -16522,6 +16518,9 @@
       <c r="H226" t="s">
         <v>740</v>
       </c>
+      <c r="J226" s="3" t="s">
+        <v>2193</v>
+      </c>
       <c r="K226" t="s">
         <v>985</v>
       </c>
@@ -16543,11 +16542,8 @@
       <c r="Q226" s="3" t="s">
         <v>1432</v>
       </c>
-      <c r="R226" s="3" t="s">
-        <v>2193</v>
-      </c>
-    </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A227" s="22">
         <v>1118</v>
       </c>
@@ -16589,7 +16585,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A228" s="22">
         <v>1119</v>
       </c>
@@ -16628,7 +16624,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A229" s="22">
         <v>1120</v>
       </c>
@@ -16670,7 +16666,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A230" s="22">
         <v>1121</v>
       </c>
@@ -16712,7 +16708,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="231" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="22">
         <v>1122</v>
       </c>
@@ -16754,7 +16750,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A232" s="22">
         <v>1123</v>
       </c>
@@ -16796,7 +16792,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A233" s="22">
         <v>1124</v>
       </c>
@@ -16838,7 +16834,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A234" s="22">
         <v>1125</v>
       </c>
@@ -16880,7 +16876,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="235" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="26">
         <v>1126</v>
       </c>
@@ -16922,7 +16918,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="236" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="22">
         <v>1127</v>
       </c>
@@ -16967,7 +16963,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A237" s="22">
         <v>1127</v>
       </c>
@@ -17001,7 +16997,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A238" s="22">
         <v>1127</v>
       </c>
@@ -17035,7 +17031,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A239" s="22">
         <v>1128</v>
       </c>
@@ -17077,7 +17073,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A240" s="22">
         <v>1129</v>
       </c>
@@ -17116,7 +17112,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="241" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="22">
         <v>1130</v>
       </c>
@@ -17158,7 +17154,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="242" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="22">
         <v>1131</v>
       </c>
@@ -17200,7 +17196,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A243" s="22">
         <v>1131</v>
       </c>
@@ -17234,7 +17230,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A244" s="22">
         <v>1131</v>
       </c>
@@ -17268,7 +17264,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A245" s="22">
         <v>1132</v>
       </c>
@@ -17310,7 +17306,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="246" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="26">
         <v>1133</v>
       </c>
@@ -17333,6 +17329,9 @@
       <c r="H246" t="s">
         <v>756</v>
       </c>
+      <c r="J246" s="3" t="s">
+        <v>2194</v>
+      </c>
       <c r="K246" t="s">
         <v>996</v>
       </c>
@@ -17351,11 +17350,8 @@
       <c r="P246" s="3" t="s">
         <v>1306</v>
       </c>
-      <c r="R246" s="3" t="s">
-        <v>2194</v>
-      </c>
-    </row>
-    <row r="247" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="22">
         <v>1134</v>
       </c>
@@ -17378,6 +17374,9 @@
       <c r="H247" t="s">
         <v>757</v>
       </c>
+      <c r="J247" s="3" t="s">
+        <v>2195</v>
+      </c>
       <c r="K247" t="s">
         <v>997</v>
       </c>
@@ -17396,11 +17395,8 @@
       <c r="Q247" s="3" t="s">
         <v>1445</v>
       </c>
-      <c r="R247" s="3" t="s">
-        <v>2195</v>
-      </c>
-    </row>
-    <row r="248" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="22">
         <v>1135</v>
       </c>
@@ -17423,6 +17419,9 @@
       <c r="H248" t="s">
         <v>758</v>
       </c>
+      <c r="J248" s="3" t="s">
+        <v>2195</v>
+      </c>
       <c r="K248" t="s">
         <v>997</v>
       </c>
@@ -17441,11 +17440,8 @@
       <c r="Q248" s="3" t="s">
         <v>1446</v>
       </c>
-      <c r="R248" s="3" t="s">
-        <v>2195</v>
-      </c>
-    </row>
-    <row r="249" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="22">
         <v>1136</v>
       </c>
@@ -17490,7 +17486,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A250" s="22">
         <v>1136</v>
       </c>
@@ -17524,7 +17520,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A251" s="22">
         <v>1136</v>
       </c>
@@ -17558,7 +17554,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="252" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="22">
         <v>1137</v>
       </c>
@@ -17600,7 +17596,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A253" s="22">
         <v>1138</v>
       </c>
@@ -17642,7 +17638,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="254" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="22">
         <v>1139</v>
       </c>
@@ -17687,7 +17683,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A255" s="22">
         <v>1139</v>
       </c>
@@ -17721,7 +17717,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A256" s="22">
         <v>1139</v>
       </c>
@@ -17755,7 +17751,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A257" s="22">
         <v>1140</v>
       </c>
@@ -17797,7 +17793,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="258" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="22">
         <v>1141</v>
       </c>
@@ -17839,7 +17835,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A259" s="22">
         <v>1141</v>
       </c>
@@ -17873,7 +17869,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A260" s="22">
         <v>1141</v>
       </c>
@@ -17907,7 +17903,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A261" s="22">
         <v>1142</v>
       </c>
@@ -17946,7 +17942,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A262" s="22">
         <v>1143</v>
       </c>
@@ -17988,7 +17984,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="263" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="22">
         <v>1144</v>
       </c>
@@ -18011,6 +18007,9 @@
       <c r="H263" t="s">
         <v>767</v>
       </c>
+      <c r="J263" s="3" t="s">
+        <v>2196</v>
+      </c>
       <c r="K263" t="s">
         <v>1002</v>
       </c>
@@ -18029,11 +18028,8 @@
       <c r="Q263" s="3" t="s">
         <v>1455</v>
       </c>
-      <c r="R263" s="3" t="s">
-        <v>2196</v>
-      </c>
-    </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A264" s="22">
         <v>1145</v>
       </c>
@@ -18075,7 +18071,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="265" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="22">
         <v>1146</v>
       </c>
@@ -18120,7 +18116,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A266" s="22">
         <v>1146</v>
       </c>
@@ -18154,7 +18150,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A267" s="22">
         <v>1146</v>
       </c>
@@ -18188,7 +18184,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A268" s="22">
         <v>1147</v>
       </c>
@@ -18227,7 +18223,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A269" s="22">
         <v>1148</v>
       </c>
@@ -18266,7 +18262,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A270" s="22">
         <v>1149</v>
       </c>
@@ -18305,7 +18301,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A271" s="22">
         <v>1150</v>
       </c>
@@ -18344,7 +18340,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A272" s="22">
         <v>1151</v>
       </c>
@@ -18383,7 +18379,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A273" s="22">
         <v>1152</v>
       </c>
@@ -18422,7 +18418,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A274" s="22">
         <v>1153</v>
       </c>
@@ -18464,7 +18460,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A275" s="22">
         <v>1154</v>
       </c>
@@ -18506,7 +18502,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A276" s="22">
         <v>1155</v>
       </c>
@@ -18548,7 +18544,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="277" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="22">
         <v>1156</v>
       </c>
@@ -18571,6 +18567,9 @@
       <c r="H277" t="s">
         <v>779</v>
       </c>
+      <c r="J277" s="3" t="s">
+        <v>2196</v>
+      </c>
       <c r="K277" t="s">
         <v>1005</v>
       </c>
@@ -18586,11 +18585,8 @@
       <c r="O277" t="s">
         <v>1747</v>
       </c>
-      <c r="R277" s="3" t="s">
-        <v>2196</v>
-      </c>
-    </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A278" s="22">
         <v>1157</v>
       </c>
@@ -18635,7 +18631,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A279" s="22">
         <v>1158</v>
       </c>
@@ -18674,7 +18670,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A280" s="22">
         <v>1159</v>
       </c>
@@ -18713,7 +18709,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="281" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="22">
         <v>1160</v>
       </c>
@@ -18758,7 +18754,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A282" s="22">
         <v>1161</v>
       </c>
@@ -18800,7 +18796,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A283" s="22">
         <v>1162</v>
       </c>
@@ -18842,7 +18838,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="284" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="22">
         <v>1163</v>
       </c>
@@ -18865,6 +18861,9 @@
       <c r="H284" t="s">
         <v>786</v>
       </c>
+      <c r="J284" s="3" t="s">
+        <v>2196</v>
+      </c>
       <c r="K284" t="s">
         <v>1010</v>
       </c>
@@ -18886,11 +18885,8 @@
       <c r="Q284" s="3" t="s">
         <v>1473</v>
       </c>
-      <c r="R284" s="3" t="s">
-        <v>2196</v>
-      </c>
-    </row>
-    <row r="285" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="285" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" s="22">
         <v>1164</v>
       </c>
@@ -18913,6 +18909,9 @@
       <c r="H285" t="s">
         <v>787</v>
       </c>
+      <c r="J285" s="3" t="s">
+        <v>2196</v>
+      </c>
       <c r="K285" t="s">
         <v>1010</v>
       </c>
@@ -18931,11 +18930,8 @@
       <c r="Q285" s="3" t="s">
         <v>1474</v>
       </c>
-      <c r="R285" s="3" t="s">
-        <v>2196</v>
-      </c>
-    </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A286" s="22">
         <v>1165</v>
       </c>
@@ -18980,7 +18976,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A287" s="22">
         <v>1166</v>
       </c>
@@ -19025,7 +19021,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A288" s="22">
         <v>1167</v>
       </c>
@@ -19070,7 +19066,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A289" s="22">
         <v>1168</v>
       </c>
@@ -19115,7 +19111,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A290" s="22">
         <v>1169</v>
       </c>
@@ -19157,7 +19153,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A291" s="22">
         <v>1170</v>
       </c>
@@ -19196,7 +19192,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A292" s="22">
         <v>1171</v>
       </c>
@@ -19235,7 +19231,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A293" s="22">
         <v>1172</v>
       </c>
@@ -19280,7 +19276,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="294" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="22">
         <v>1173</v>
       </c>
@@ -19322,7 +19318,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A295" s="22">
         <v>1174</v>
       </c>
@@ -19364,7 +19360,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="296" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A296" s="22">
         <v>1175</v>
       </c>
@@ -19406,7 +19402,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="297" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="22">
         <v>1176</v>
       </c>
@@ -19448,7 +19444,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="298" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="22">
         <v>1177</v>
       </c>
@@ -19490,7 +19486,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A299" s="22">
         <v>1178</v>
       </c>
@@ -19532,7 +19528,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="300" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="22">
         <v>1179</v>
       </c>
@@ -19574,7 +19570,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A301" s="22">
         <v>1180</v>
       </c>
@@ -19597,6 +19593,9 @@
       <c r="H301" t="s">
         <v>803</v>
       </c>
+      <c r="J301" s="3" t="s">
+        <v>2197</v>
+      </c>
       <c r="K301" t="s">
         <v>1020</v>
       </c>
@@ -19615,11 +19614,8 @@
       <c r="Q301" s="3" t="s">
         <v>1490</v>
       </c>
-      <c r="R301" s="3" t="s">
-        <v>2197</v>
-      </c>
-    </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A302" s="22">
         <v>1181</v>
       </c>
@@ -19642,6 +19638,9 @@
       <c r="H302" t="s">
         <v>804</v>
       </c>
+      <c r="J302" s="3" t="s">
+        <v>2197</v>
+      </c>
       <c r="K302" t="s">
         <v>1020</v>
       </c>
@@ -19654,11 +19653,8 @@
       <c r="O302" t="s">
         <v>1768</v>
       </c>
-      <c r="R302" s="3" t="s">
-        <v>2197</v>
-      </c>
-    </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A303" s="22">
         <v>1182</v>
       </c>
@@ -19703,7 +19699,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A304" s="22">
         <v>1183</v>
       </c>
@@ -19748,7 +19744,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A305" s="22">
         <v>1184</v>
       </c>
@@ -19790,7 +19786,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A306" s="22">
         <v>1185</v>
       </c>
@@ -19832,7 +19828,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A307" s="22">
         <v>1186</v>
       </c>
@@ -19877,7 +19873,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A308" s="22">
         <v>1186</v>
       </c>
@@ -19911,7 +19907,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A309" s="22">
         <v>1186</v>
       </c>
@@ -19945,7 +19941,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="310" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="22">
         <v>1187</v>
       </c>
@@ -19968,6 +19964,9 @@
       <c r="H310" t="s">
         <v>810</v>
       </c>
+      <c r="J310" s="3" t="s">
+        <v>2198</v>
+      </c>
       <c r="K310">
         <v>1976</v>
       </c>
@@ -19986,11 +19985,8 @@
       <c r="Q310" s="3" t="s">
         <v>1496</v>
       </c>
-      <c r="R310" s="3" t="s">
-        <v>2198</v>
-      </c>
-    </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A311" s="22">
         <v>1188</v>
       </c>
@@ -20032,7 +20028,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A312" s="22">
         <v>1189</v>
       </c>
@@ -20068,7 +20064,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="313" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A313" s="22">
         <v>1190</v>
       </c>
@@ -20110,7 +20106,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A314" s="22">
         <v>1190</v>
       </c>
@@ -20144,7 +20140,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A315" s="22">
         <v>1190</v>
       </c>
@@ -20178,7 +20174,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A316" s="22">
         <v>1191</v>
       </c>
@@ -20214,7 +20210,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="317" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A317" s="22">
         <v>1192</v>
       </c>
@@ -20256,7 +20252,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="318" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A318" s="22">
         <v>1193</v>
       </c>
@@ -20298,7 +20294,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="319" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A319" s="22">
         <v>1194</v>
       </c>
@@ -20340,7 +20336,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="320" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A320" s="22">
         <v>1195</v>
       </c>
@@ -20363,6 +20359,9 @@
       <c r="H320" t="s">
         <v>812</v>
       </c>
+      <c r="J320" s="3" t="s">
+        <v>2199</v>
+      </c>
       <c r="K320" t="s">
         <v>1026</v>
       </c>
@@ -20377,9 +20376,6 @@
       </c>
       <c r="O320" t="s">
         <v>1763</v>
-      </c>
-      <c r="R320" s="3" t="s">
-        <v>2199</v>
       </c>
     </row>
     <row r="321" spans="1:17" x14ac:dyDescent="0.25">
@@ -21011,7 +21007,7 @@
         <v>1498</v>
       </c>
     </row>
-    <row r="337" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A337" s="22">
         <v>1210</v>
       </c>
@@ -21050,7 +21046,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="338" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A338" s="22">
         <v>1211</v>
       </c>
@@ -21089,7 +21085,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A339" s="22">
         <v>1212</v>
       </c>
@@ -21131,7 +21127,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="340" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A340" s="22">
         <v>1213</v>
       </c>
@@ -21173,7 +21169,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="341" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A341" s="22">
         <v>1214</v>
       </c>
@@ -21212,7 +21208,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="342" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A342" s="22">
         <v>1215</v>
       </c>
@@ -21251,7 +21247,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="343" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A343" s="22">
         <v>1216</v>
       </c>
@@ -21290,7 +21286,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="344" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A344" s="22">
         <v>1217</v>
       </c>
@@ -21329,7 +21325,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="345" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A345" s="22">
         <v>1218</v>
       </c>
@@ -21371,7 +21367,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="346" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" s="22">
         <v>1219</v>
       </c>
@@ -21394,6 +21390,9 @@
       <c r="H346" t="s">
         <v>836</v>
       </c>
+      <c r="J346" s="3" t="s">
+        <v>2200</v>
+      </c>
       <c r="K346" t="s">
         <v>1041</v>
       </c>
@@ -21409,11 +21408,8 @@
       <c r="O346" t="s">
         <v>1772</v>
       </c>
-      <c r="R346" s="3" t="s">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="347" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A347" s="22">
         <v>1220</v>
       </c>
@@ -21452,7 +21448,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="348" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A348" s="22">
         <v>1221</v>
       </c>
@@ -21491,7 +21487,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="349" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A349" s="22">
         <v>1222</v>
       </c>
@@ -21530,7 +21526,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="350" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A350" s="22">
         <v>1223</v>
       </c>
@@ -21553,6 +21549,9 @@
       <c r="H350" t="s">
         <v>840</v>
       </c>
+      <c r="J350" s="3" t="s">
+        <v>2201</v>
+      </c>
       <c r="K350" t="s">
         <v>1043</v>
       </c>
@@ -21568,11 +21567,8 @@
       <c r="O350" t="s">
         <v>1763</v>
       </c>
-      <c r="R350" s="3" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="351" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A351" s="22">
         <v>1224</v>
       </c>
@@ -21611,7 +21607,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="352" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A352" s="22">
         <v>1225</v>
       </c>
@@ -21647,7 +21643,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="353" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A353" s="22">
         <v>1226</v>
       </c>
@@ -21686,7 +21682,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="354" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A354" s="22">
         <v>1227</v>
       </c>
@@ -21709,6 +21705,9 @@
       <c r="H354" t="s">
         <v>843</v>
       </c>
+      <c r="J354" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K354" t="s">
         <v>1045</v>
       </c>
@@ -21724,11 +21723,8 @@
       <c r="O354" t="s">
         <v>1763</v>
       </c>
-      <c r="R354" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="355" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="355" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A355" s="22">
         <v>1228</v>
       </c>
@@ -21751,6 +21747,9 @@
       <c r="H355" t="s">
         <v>844</v>
       </c>
+      <c r="J355" s="3" t="s">
+        <v>2200</v>
+      </c>
       <c r="K355" t="s">
         <v>1046</v>
       </c>
@@ -21766,11 +21765,8 @@
       <c r="O355" t="s">
         <v>1743</v>
       </c>
-      <c r="R355" s="3" t="s">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="356" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="356" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A356" s="22">
         <v>1229</v>
       </c>
@@ -21809,7 +21805,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="357" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A357" s="22">
         <v>1230</v>
       </c>
@@ -21845,7 +21841,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="358" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A358" s="22">
         <v>1231</v>
       </c>
@@ -21868,6 +21864,9 @@
       <c r="H358" t="s">
         <v>847</v>
       </c>
+      <c r="J358" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K358" t="s">
         <v>1049</v>
       </c>
@@ -21889,11 +21888,8 @@
       <c r="Q358" s="3" t="s">
         <v>1219</v>
       </c>
-      <c r="R358" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="359" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A359" s="22">
         <v>1231</v>
       </c>
@@ -21927,7 +21923,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="360" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A360" s="22">
         <v>1231</v>
       </c>
@@ -21961,7 +21957,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="361" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A361" s="22">
         <v>1232</v>
       </c>
@@ -21984,6 +21980,9 @@
       <c r="H361" t="s">
         <v>847</v>
       </c>
+      <c r="J361" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K361" t="s">
         <v>1049</v>
       </c>
@@ -22005,11 +22004,8 @@
       <c r="Q361" s="3" t="s">
         <v>1219</v>
       </c>
-      <c r="R361" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="362" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A362" s="22">
         <v>1232</v>
       </c>
@@ -22043,7 +22039,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="363" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A363" s="22">
         <v>1232</v>
       </c>
@@ -22077,7 +22073,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="364" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A364" s="22">
         <v>1233</v>
       </c>
@@ -22116,7 +22112,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="365" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A365" s="22">
         <v>1234</v>
       </c>
@@ -22158,7 +22154,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="366" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A366" s="22">
         <v>1235</v>
       </c>
@@ -22200,7 +22196,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="367" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A367" s="22">
         <v>1236</v>
       </c>
@@ -22236,7 +22232,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="368" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A368" s="22">
         <v>1237</v>
       </c>
@@ -22272,7 +22268,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="369" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A369" s="22">
         <v>1238</v>
       </c>
@@ -22308,7 +22304,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="370" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A370" s="22">
         <v>1239</v>
       </c>
@@ -22347,7 +22343,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="371" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A371" s="22">
         <v>1240</v>
       </c>
@@ -22383,7 +22379,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="372" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A372" s="22">
         <v>1240</v>
       </c>
@@ -22417,7 +22413,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="373" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A373" s="22">
         <v>1240</v>
       </c>
@@ -22451,7 +22447,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="374" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A374" s="22">
         <v>1241</v>
       </c>
@@ -22490,7 +22486,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="375" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A375" s="22">
         <v>1242</v>
       </c>
@@ -22526,7 +22522,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="376" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A376" s="22">
         <v>1243</v>
       </c>
@@ -22565,7 +22561,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="377" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A377" s="22">
         <v>1244</v>
       </c>
@@ -22604,7 +22600,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="378" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A378" s="22">
         <v>1245</v>
       </c>
@@ -22643,7 +22639,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="379" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A379" s="22">
         <v>1246</v>
       </c>
@@ -22682,7 +22678,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="380" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A380" s="22">
         <v>1247</v>
       </c>
@@ -22721,7 +22717,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="381" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A381" s="22">
         <v>1248</v>
       </c>
@@ -22744,6 +22740,9 @@
       <c r="H381" t="s">
         <v>860</v>
       </c>
+      <c r="J381" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K381" t="s">
         <v>1062</v>
       </c>
@@ -22762,11 +22761,8 @@
       <c r="P381" s="3" t="s">
         <v>1319</v>
       </c>
-      <c r="R381" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="382" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="382" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A382" s="22">
         <v>1249</v>
       </c>
@@ -22789,6 +22785,9 @@
       <c r="H382" t="s">
         <v>861</v>
       </c>
+      <c r="J382" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K382" t="s">
         <v>1063</v>
       </c>
@@ -22804,11 +22803,8 @@
       <c r="O382" t="s">
         <v>1774</v>
       </c>
-      <c r="R382" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="383" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="383" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A383" s="22">
         <v>1250</v>
       </c>
@@ -22831,6 +22827,9 @@
       <c r="H383" t="s">
         <v>862</v>
       </c>
+      <c r="J383" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K383" t="s">
         <v>1064</v>
       </c>
@@ -22843,11 +22842,8 @@
       <c r="O383" t="s">
         <v>1751</v>
       </c>
-      <c r="R383" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="384" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="384" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A384" s="22">
         <v>1251</v>
       </c>
@@ -22883,7 +22879,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="385" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A385" s="22">
         <v>1252</v>
       </c>
@@ -22906,6 +22902,9 @@
       <c r="H385" t="s">
         <v>863</v>
       </c>
+      <c r="J385" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K385">
         <v>1985</v>
       </c>
@@ -22921,11 +22920,8 @@
       <c r="O385" t="s">
         <v>1773</v>
       </c>
-      <c r="R385" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="386" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="386" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A386" s="22">
         <v>1253</v>
       </c>
@@ -22948,6 +22944,9 @@
       <c r="H386" t="s">
         <v>863</v>
       </c>
+      <c r="J386" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K386">
         <v>1985</v>
       </c>
@@ -22963,11 +22962,8 @@
       <c r="O386" t="s">
         <v>1773</v>
       </c>
-      <c r="R386" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="387" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A387" s="22">
         <v>1254</v>
       </c>
@@ -23003,7 +22999,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="388" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A388" s="26">
         <v>1255</v>
       </c>
@@ -23026,6 +23022,9 @@
       <c r="H388" t="s">
         <v>865</v>
       </c>
+      <c r="J388" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K388" t="s">
         <v>1066</v>
       </c>
@@ -23044,11 +23043,8 @@
       <c r="P388" s="3" t="s">
         <v>1320</v>
       </c>
-      <c r="R388" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="389" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="389" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A389" s="22">
         <v>1256</v>
       </c>
@@ -23071,6 +23067,9 @@
       <c r="H389" t="s">
         <v>866</v>
       </c>
+      <c r="J389" s="3" t="s">
+        <v>2202</v>
+      </c>
       <c r="K389" t="s">
         <v>1067</v>
       </c>
@@ -23089,11 +23088,8 @@
       <c r="Q389" s="3" t="s">
         <v>1499</v>
       </c>
-      <c r="R389" s="3" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="390" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="390" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A390" s="22">
         <v>1257</v>
       </c>
@@ -23132,7 +23128,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="391" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A391" s="22">
         <v>1258</v>
       </c>
@@ -23155,6 +23151,9 @@
       <c r="H391" t="s">
         <v>742</v>
       </c>
+      <c r="J391" s="3" t="s">
+        <v>2203</v>
+      </c>
       <c r="K391" t="s">
         <v>1069</v>
       </c>
@@ -23170,11 +23169,8 @@
       <c r="O391" t="s">
         <v>1763</v>
       </c>
-      <c r="R391" s="3" t="s">
-        <v>2203</v>
-      </c>
-    </row>
-    <row r="392" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="392" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A392" s="22">
         <v>1259</v>
       </c>
@@ -23213,7 +23209,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="393" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A393" s="22">
         <v>1260</v>
       </c>
@@ -23252,7 +23248,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="394" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A394" s="22">
         <v>1261</v>
       </c>
@@ -23294,7 +23290,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="395" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A395" s="22">
         <v>1262</v>
       </c>
@@ -23330,7 +23326,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="396" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A396" s="22">
         <v>1263</v>
       </c>
@@ -23369,7 +23365,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="397" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A397" s="22">
         <v>1264</v>
       </c>
@@ -23408,7 +23404,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="398" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A398" s="22">
         <v>1265</v>
       </c>
@@ -23447,7 +23443,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="399" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A399" s="22">
         <v>1265</v>
       </c>
@@ -23481,7 +23477,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="400" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A400" s="22">
         <v>1265</v>
       </c>
@@ -24075,7 +24071,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="417" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A417" s="22">
         <v>1274</v>
       </c>
@@ -24114,7 +24110,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="418" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A418" s="22">
         <v>1274</v>
       </c>
@@ -24148,7 +24144,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="419" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A419" s="22">
         <v>1274</v>
       </c>
@@ -24182,7 +24178,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="420" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A420" s="22">
         <v>1275</v>
       </c>
@@ -24221,7 +24217,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="421" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A421" s="22">
         <v>1276</v>
       </c>
@@ -24260,7 +24256,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="422" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A422" s="22">
         <v>1277</v>
       </c>
@@ -24299,7 +24295,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="423" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A423" s="22">
         <v>1278</v>
       </c>
@@ -24329,7 +24325,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="424" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A424" s="22">
         <v>1278</v>
       </c>
@@ -24357,7 +24353,7 @@
       <c r="M424" s="23"/>
       <c r="O424"/>
     </row>
-    <row r="425" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A425" s="22">
         <v>1278</v>
       </c>
@@ -24385,7 +24381,7 @@
       <c r="M425" s="23"/>
       <c r="O425"/>
     </row>
-    <row r="426" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A426" s="22">
         <v>1279</v>
       </c>
@@ -24421,7 +24417,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="427" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A427" s="22">
         <v>1280</v>
       </c>
@@ -24444,6 +24440,9 @@
       <c r="H427" t="s">
         <v>884</v>
       </c>
+      <c r="J427" s="3" t="s">
+        <v>2192</v>
+      </c>
       <c r="K427" t="s">
         <v>1075</v>
       </c>
@@ -24459,11 +24458,8 @@
       <c r="Q427" s="3" t="s">
         <v>1500</v>
       </c>
-      <c r="R427" s="3" t="s">
-        <v>2192</v>
-      </c>
-    </row>
-    <row r="428" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="428" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A428" s="22">
         <v>1280</v>
       </c>
@@ -24497,7 +24493,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="429" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A429" s="22">
         <v>1280</v>
       </c>
@@ -24531,7 +24527,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="430" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A430" s="22">
         <v>1281</v>
       </c>
@@ -24554,6 +24550,9 @@
       <c r="H430" t="s">
         <v>885</v>
       </c>
+      <c r="J430" s="3" t="s">
+        <v>2192</v>
+      </c>
       <c r="K430" t="s">
         <v>1075</v>
       </c>
@@ -24575,11 +24574,8 @@
       <c r="Q430" s="3" t="s">
         <v>1501</v>
       </c>
-      <c r="R430" s="3" t="s">
-        <v>2192</v>
-      </c>
-    </row>
-    <row r="431" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="431" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A431" s="22">
         <v>1281</v>
       </c>
@@ -24613,7 +24609,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="432" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A432" s="22">
         <v>1281</v>
       </c>
@@ -26836,7 +26832,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
@@ -26869,27 +26865,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
-          </x14:formula1>
-          <xm:sqref>J1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>R1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
             <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
           </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
+          <xm:sqref>I1:J1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>

</xml_diff>